<commit_message>
rename mutag to imdbb on premodel integration
</commit_message>
<xml_diff>
--- a/logs/Logs.xlsx
+++ b/logs/Logs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlan\Documents\Lab\Graph subgraph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sclab\Documents\Lab\Subgraph and partitioning method\graph-ap\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA3DEBF-5CE1-4FD2-9147-DCE74B59A9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA5CF1-80A8-449D-9F8F-FE58E8B4E613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2BDFC8CA-ADA5-44E8-BB01-FF36EC6D4B04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{2BDFC8CA-ADA5-44E8-BB01-FF36EC6D4B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Fold" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment Fold" sheetId="2" r:id="rId2"/>
+    <sheet name="Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,12 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="44">
   <si>
     <t>Base</t>
   </si>
@@ -152,12 +148,34 @@
   <si>
     <t>Fold 10/10</t>
   </si>
+  <si>
+    <t>Fold Acc</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>Fold</t>
+  </si>
+  <si>
+    <t>With Subgraph
+(concat)</t>
+  </si>
+  <si>
+    <t>Base (GCN)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +199,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -198,14 +224,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5C66DA-43D9-447B-9EB7-5601E42E1AB5}">
-  <dimension ref="A1:L122"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="266" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,17 +584,20 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -566,8 +622,12 @@
       <c r="H3">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f>H13</f>
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -592,8 +652,12 @@
       <c r="H4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f>H25</f>
+        <v>0.6333359999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -618,8 +682,12 @@
       <c r="H5">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f>H38</f>
+        <v>0.6333359999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -644,8 +712,12 @@
       <c r="H6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <f>H50</f>
+        <v>0.68666400000000016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -670,8 +742,12 @@
       <c r="H7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f>H62</f>
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -696,8 +772,12 @@
       <c r="H8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <f>H74</f>
+        <v>0.79333600000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -722,8 +802,12 @@
       <c r="H9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f>H86</f>
+        <v>0.52666400000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -748,8 +832,12 @@
       <c r="H10">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <f>H98</f>
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -774,8 +862,12 @@
       <c r="H11">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <f>H110</f>
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -800,27 +892,37 @@
       <c r="H12">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <f>H122</f>
+        <v>0.68666400000000016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H13">
         <f>AVERAGE(H3:H12)</f>
         <v>0.57999999999999985</v>
       </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
       <c r="K13">
-        <f>AVERAGE(H13,H25,H38,H50,H62,H74,H86,H98,H110,H122)</f>
+        <f>AVERAGE(K3:K12)</f>
         <v>0.628</v>
       </c>
-      <c r="L13">
-        <f>_xlfn.STDEV.P(H13,H25,H38,H50,H62,H74,H86,H98,H110,H122)</f>
-        <v>7.3321793060453264E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <f>_xlfn.STDEV.P(K3:K12)</f>
+        <v>7.3321793060453264E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -846,7 +948,7 @@
         <v>0.33333000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3262,25 +3364,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB8A0B2-D368-4C74-9B31-80C4B964A068}">
-  <dimension ref="A1:L121"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3305,8 +3410,12 @@
       <c r="H3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f>H13</f>
+        <v>0.59999999999999987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3331,8 +3440,12 @@
       <c r="H4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f>H25</f>
+        <v>0.6333359999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3357,8 +3470,12 @@
       <c r="H5">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f>H37</f>
+        <v>0.6333359999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3383,8 +3500,12 @@
       <c r="H6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <f>H49</f>
+        <v>0.68666400000000016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3409,8 +3530,12 @@
       <c r="H7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f>H61</f>
+        <v>0.59999999999999987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3435,8 +3560,12 @@
       <c r="H8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <f>H73</f>
+        <v>0.79333600000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -3461,8 +3590,12 @@
       <c r="H9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f>H85</f>
+        <v>0.53333000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3487,8 +3620,12 @@
       <c r="H10">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <f>H97</f>
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -3513,8 +3650,12 @@
       <c r="H11">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <f>H109</f>
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3539,27 +3680,37 @@
       <c r="H12">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <f>H121</f>
+        <v>0.68666400000000016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H13">
         <f>AVERAGE(H3:H12)</f>
         <v>0.59999999999999987</v>
       </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
       <c r="K13">
-        <f>AVERAGE(H13,H25,H37,H49,H61,H73,H85,H97,H109,H121)</f>
+        <f>AVERAGE(K3:K12)</f>
         <v>0.63266660000000008</v>
       </c>
-      <c r="L13">
-        <f>_xlfn.STDEV.P(H13,H25,H37,H49,H61,H73,H85,H97,H109,H121)</f>
-        <v>7.0140220861071675E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <f>_xlfn.STDEV.P(K3:K12)</f>
+        <v>7.0140220861071675E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -3585,7 +3736,7 @@
         <v>0.33333000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -5996,4 +6147,171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE9C9D3-2ECC-4B93-BCE1-A0567D2F61B9}">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.57999999999999985</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.59999999999999987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.6333359999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.6333359999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.6333359999999999</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.6333359999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.68666400000000016</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.68666400000000016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.57999999999999985</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.59999999999999987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.79333600000000004</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.79333600000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.52666400000000002</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.53333000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.57999999999999985</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.57999999999999985</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.57999999999999985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.68666400000000016</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.68666400000000016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="6">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.628</v>
+      </c>
+      <c r="C13" s="7">
+        <f>AVERAGE(C3:C12)</f>
+        <v>0.63266660000000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="6">
+        <f>_xlfn.STDEV.P(B3:B12)</f>
+        <v>7.3321793060453264E-2</v>
+      </c>
+      <c r="C14" s="6">
+        <f>_xlfn.STDEV.P(C3:C12)</f>
+        <v>7.0140220861071675E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>